<commit_message>
buttons.xlsx now allow multiple users
Added column for "user" which would only apply for selected user.
</commit_message>
<xml_diff>
--- a/inputs/buttons.xlsx
+++ b/inputs/buttons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuan\Documents\GitHub\tuans_world\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tt04658\OneDrive - The Hartford\Documents\Github\tuans_world\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1A17A6-1A76-43D9-8447-4D708FE8424A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9901AE-D4A9-40D6-A254-179760D52323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{F53843A5-4C8D-4DE0-AFBD-DDF1A7BEE99F}"/>
+    <workbookView xWindow="29835" yWindow="4545" windowWidth="20490" windowHeight="10920" xr2:uid="{F53843A5-4C8D-4DE0-AFBD-DDF1A7BEE99F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>Button</t>
   </si>
@@ -48,48 +48,74 @@
     <t>VSCode</t>
   </si>
   <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>Tuan's World</t>
+  </si>
+  <si>
+    <t>Downloads</t>
+  </si>
+  <si>
+    <t>hydro-py</t>
+  </si>
+  <si>
+    <t>C:\Users\TT04658\Downloads\</t>
+  </si>
+  <si>
+    <t>C:\Users\TT04658\Documents\GitHub\vsc_tuansworld.bat</t>
+  </si>
+  <si>
+    <t>C:\Users\tuan\OneDrive\Desktop\iCRM.bat</t>
+  </si>
+  <si>
+    <t>C:\Users\tuan\OneDrive\Desktop\HydroPie Flask.bat</t>
+  </si>
+  <si>
     <t>C:\Users\tuan\Documents\GitHub\iCRM</t>
   </si>
   <si>
     <t>C:\Users\tuan\Documents\GitHub\tuans_world</t>
   </si>
   <si>
-    <t>Folder</t>
+    <t>C:\Users\tuan\Downloads\</t>
   </si>
   <si>
     <t>C:\Users\tuan\Documents\GitHub\vsc_icrm.bat</t>
   </si>
   <si>
-    <t>C:\Users\tuan\OneDrive\Desktop\iCRM.bat</t>
-  </si>
-  <si>
-    <t>C:\Users\tuan\OneDrive\Desktop\HydroPie Flask.bat</t>
-  </si>
-  <si>
     <t>C:\Users\tuan\Documents\GitHub\vsc_tuansworld.bat</t>
   </si>
   <si>
-    <t>Tuan's World</t>
-  </si>
-  <si>
-    <t>Downloads</t>
-  </si>
-  <si>
-    <t>C:\Users\tuan\Downloads\</t>
-  </si>
-  <si>
-    <t>hydro-py</t>
-  </si>
-  <si>
     <t>C:\Users\tuan\Documents\GitHub\vsc_hydropy.bat</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>tuan</t>
+  </si>
+  <si>
+    <t>TT04658</t>
+  </si>
+  <si>
+    <t>C:\Users\tt04658\OneDrive - The Hartford\Documents\Github\tuans_world</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,9 +149,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BAA9C9-76B0-469F-9CFA-41DD7A7485DD}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,18 +480,21 @@
     <col min="3" max="3" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -472,10 +502,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -483,43 +516,55 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -527,32 +572,84 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major changes for customization
Change buttons file, change icon. Settings file.
</commit_message>
<xml_diff>
--- a/inputs/buttons.xlsx
+++ b/inputs/buttons.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tt04658\OneDrive - The Hartford\Documents\Github\tuans_world\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuan\Documents\GitHub\tuans_world\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9901AE-D4A9-40D6-A254-179760D52323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307C589D-13FC-4C1C-BA9F-FB4554FD6A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29835" yWindow="4545" windowWidth="20490" windowHeight="10920" xr2:uid="{F53843A5-4C8D-4DE0-AFBD-DDF1A7BEE99F}"/>
+    <workbookView xWindow="5070" yWindow="3090" windowWidth="21600" windowHeight="11295" xr2:uid="{F53843A5-4C8D-4DE0-AFBD-DDF1A7BEE99F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Buttons" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Button</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>C:\Users\tt04658\OneDrive - The Hartford\Documents\Github\tuans_world</t>
+  </si>
+  <si>
+    <t>QtDesigner</t>
+  </si>
+  <si>
+    <t>C:\Users\tuan\Anaconda3\envs\icrm\Scripts\designer.exe</t>
   </si>
 </sst>
 </file>
@@ -123,18 +129,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,9 +149,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -467,30 +466,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BAA9C9-76B0-469F-9CFA-41DD7A7485DD}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="3" max="3" width="69.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -524,13 +523,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -538,27 +537,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -566,13 +565,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -580,13 +579,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -594,13 +593,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -608,27 +607,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -636,15 +635,29 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>